<commit_message>
update proof of proper secret
</commit_message>
<xml_diff>
--- a/ascii_codes_refs.xlsx
+++ b/ascii_codes_refs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\code\fruity-lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBCBA8C-2F9E-4038-A1B9-E3BF8C1B30CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04111CC1-5C2E-4CCA-BEE0-1BC1596CFE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{8F7FA4C2-AC18-4BC9-8412-504136628C51}"/>
   </bookViews>
@@ -1847,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7A31D4-123F-4DA1-8689-A500831D64FB}">
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92:D95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1890,7 +1890,7 @@
         <v>87</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D16" si="0">C3&amp;","&amp;" // "&amp;B3</f>
+        <f t="shared" ref="D3:D66" si="0">C3&amp;","&amp;" // "&amp;B3</f>
         <v>0x253dc95d528415ea2b5fa563891bf3af151bc2576d1bda92f57047575fb86874, // " double quotation</v>
       </c>
     </row>
@@ -2100,8 +2100,8 @@
         <v>101</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D3:D66" si="1">C17&amp;","</f>
-        <v>0x1e526c4a192f3f6a79f85b4da6a98ba8ecc091bb486d1b45a3ff24ce3426c9b9,</v>
+        <f t="shared" si="0"/>
+        <v>0x1e526c4a192f3f6a79f85b4da6a98ba8ecc091bb486d1b45a3ff24ce3426c9b9, // 0</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" thickBot="1">
@@ -2115,8 +2115,8 @@
         <v>102</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0b6b02147b74321d00aca053627f131e5be0dc4b13163f6d335a8071a0f95261,</v>
+        <f t="shared" si="0"/>
+        <v>0x0b6b02147b74321d00aca053627f131e5be0dc4b13163f6d335a8071a0f95261, // 1</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" thickBot="1">
@@ -2130,8 +2130,8 @@
         <v>103</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="1"/>
-        <v>0x01388b9a8a054cc2d19939ea0c8bca387d9089244d78fb5da96a8a961945ac08,</v>
+        <f t="shared" si="0"/>
+        <v>0x01388b9a8a054cc2d19939ea0c8bca387d9089244d78fb5da96a8a961945ac08, // 2</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" thickBot="1">
@@ -2145,8 +2145,8 @@
         <v>104</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="1"/>
-        <v>0x034fc2eff5ea29664523402aec82d39bae64c8120c1f30dac99ff24a73eb8ab6,</v>
+        <f t="shared" si="0"/>
+        <v>0x034fc2eff5ea29664523402aec82d39bae64c8120c1f30dac99ff24a73eb8ab6, // 3</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" thickBot="1">
@@ -2160,8 +2160,8 @@
         <v>105</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="1"/>
-        <v>0x21141ff50ffa184999b70873c6d2e55573ca58d60245ac846fa96154989e5254,</v>
+        <f t="shared" si="0"/>
+        <v>0x21141ff50ffa184999b70873c6d2e55573ca58d60245ac846fa96154989e5254, // 4</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" thickBot="1">
@@ -2175,8 +2175,8 @@
         <v>106</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="1"/>
-        <v>0x161f58fa6bc3d4d844c272c4feab38804265785e63a6e2f3db48a240d460c2ca,</v>
+        <f t="shared" si="0"/>
+        <v>0x161f58fa6bc3d4d844c272c4feab38804265785e63a6e2f3db48a240d460c2ca, // 5</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" thickBot="1">
@@ -2190,8 +2190,8 @@
         <v>107</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2c8fcca887aadbdd7f9c858c5cdab7764d3e8defaa2dbdd7b39401f25e8c64e9,</v>
+        <f t="shared" si="0"/>
+        <v>0x2c8fcca887aadbdd7f9c858c5cdab7764d3e8defaa2dbdd7b39401f25e8c64e9, // 6</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" thickBot="1">
@@ -2205,8 +2205,8 @@
         <v>108</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1e92895d716584f84ae344a3154f62113c6a369607f3efe91443618aaae67b9a,</v>
+        <f t="shared" si="0"/>
+        <v>0x1e92895d716584f84ae344a3154f62113c6a369607f3efe91443618aaae67b9a, // 7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" thickBot="1">
@@ -2220,8 +2220,8 @@
         <v>109</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2e3a3b844eb35871138aca89a1462913730a050531ad23baa66410f25e51765d,</v>
+        <f t="shared" si="0"/>
+        <v>0x2e3a3b844eb35871138aca89a1462913730a050531ad23baa66410f25e51765d, // 8</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.5" thickBot="1">
@@ -2235,8 +2235,8 @@
         <v>110</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0b6d6f69b140cf67a585978ac44100fd7ee62bbacfd2c32c02661858af059c8e,</v>
+        <f t="shared" si="0"/>
+        <v>0x0b6d6f69b140cf67a585978ac44100fd7ee62bbacfd2c32c02661858af059c8e, // 9</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" thickBot="1">
@@ -2250,7 +2250,7 @@
         <v>111</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" ref="D27:D33" si="2">C27&amp;","&amp;" // "&amp;B27</f>
+        <f t="shared" si="0"/>
         <v>0x16d5a5f3079e061ae70adb659252fc7b7966703e5815765c6b1b89ea36092ef7, // : colon</v>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
         <v>112</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x23e9c0686bb475ed3da655407ecf1bae3d30bfe62884d7daaf6db4442cbb3fdb, // ; semicolon</v>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
         <v>113</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x03331a6c6a82d7d4d9ed03bae70d39991dacc3cd93742c6750db416d31d49bb9, // &lt; less-than sign</v>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
         <v>114</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x0e1bf9b4b0246929f34ec1d9e56b51d81428265242c07694db854e0d0563bb, // = equals sign</v>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
         <v>115</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x1d6c2e9e7876edebc7bc3bf5e747dae2cac944d13161828e9f65318b0bf90bb6, // &gt; greater-than sign</v>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
         <v>116</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x233ed04f3e71393a8b6fb3376887594247629fb429b82edea3b7a021a4fd752c, // ? question mark</v>
       </c>
     </row>
@@ -2340,7 +2340,7 @@
         <v>117</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0x19783b19011ac44704cc3b89d48689989d6a8dc7981ff95b52b26885a0bbec61, // @ at sign</v>
       </c>
     </row>
@@ -2355,8 +2355,8 @@
         <v>118</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="1"/>
-        <v>0x03cf9f0c8f51a1fd00f1a95b56620013eaa81a772152d5c44367037a902b96fe,</v>
+        <f t="shared" si="0"/>
+        <v>0x03cf9f0c8f51a1fd00f1a95b56620013eaa81a772152d5c44367037a902b96fe, // A uppercase a</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.5" thickBot="1">
@@ -2370,8 +2370,8 @@
         <v>119</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0b569b3ad90b372b5975ed9dfadd657df487df7bcf3927457c743d8d016580f1,</v>
+        <f t="shared" si="0"/>
+        <v>0x0b569b3ad90b372b5975ed9dfadd657df487df7bcf3927457c743d8d016580f1, // B uppercase b</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16.5" thickBot="1">
@@ -2385,8 +2385,8 @@
         <v>120</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0294130836e25f4fa29e92d5681128f03d7b618619c5c3b65c6352520158aa02,</v>
+        <f t="shared" si="0"/>
+        <v>0x0294130836e25f4fa29e92d5681128f03d7b618619c5c3b65c6352520158aa02, // C uppercase c</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickBot="1">
@@ -2400,8 +2400,8 @@
         <v>121</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2dc05a51251bb7788e5341fa86bc8651a48d6825025efc4077b154aad9250a2b,</v>
+        <f t="shared" si="0"/>
+        <v>0x2dc05a51251bb7788e5341fa86bc8651a48d6825025efc4077b154aad9250a2b, // D uppercase d</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickBot="1">
@@ -2415,8 +2415,8 @@
         <v>122</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="1"/>
-        <v>0x259bee2922e2fb130b6f330f3ebad5942c48ec7f7b1ad1f9ed6e8237ffed6e11,</v>
+        <f t="shared" si="0"/>
+        <v>0x259bee2922e2fb130b6f330f3ebad5942c48ec7f7b1ad1f9ed6e8237ffed6e11, // E uppercase e</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" thickBot="1">
@@ -2430,8 +2430,8 @@
         <v>123</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="1"/>
-        <v>0x07b63faa42d0459307d7ad443cb771dab0cf05465ecd78b0a0d45116dd6d4ab2,</v>
+        <f t="shared" si="0"/>
+        <v>0x07b63faa42d0459307d7ad443cb771dab0cf05465ecd78b0a0d45116dd6d4ab2, // F uppercase f</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickBot="1">
@@ -2445,8 +2445,8 @@
         <v>124</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2837a56430f12cf92151a20b0eeceb76ac6f1e26957ff74ca332c1bfc4275346,</v>
+        <f t="shared" si="0"/>
+        <v>0x2837a56430f12cf92151a20b0eeceb76ac6f1e26957ff74ca332c1bfc4275346, // G uppercase g</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickBot="1">
@@ -2460,8 +2460,8 @@
         <v>125</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0ffb5b1c4c8839581df648f1d2cd0ebd87558a1e87a456451947a3b7da3c6682,</v>
+        <f t="shared" si="0"/>
+        <v>0x0ffb5b1c4c8839581df648f1d2cd0ebd87558a1e87a456451947a3b7da3c6682, // H uppercase h</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" thickBot="1">
@@ -2475,8 +2475,8 @@
         <v>126</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>0x0e23ab9f4d077373f5dd1e06e65a42ae23c0d9856126bc131a091fa2e0bd0e1c,</v>
+        <f t="shared" si="0"/>
+        <v>0x0e23ab9f4d077373f5dd1e06e65a42ae23c0d9856126bc131a091fa2e0bd0e1c, // I uppercase i</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" thickBot="1">
@@ -2490,8 +2490,8 @@
         <v>127</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1b0c7375409814419ae60c38429d19f9c93c8fbe6c593fa0e198f60cc9036de8,</v>
+        <f t="shared" si="0"/>
+        <v>0x1b0c7375409814419ae60c38429d19f9c93c8fbe6c593fa0e198f60cc9036de8, // J uppercase j</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" thickBot="1">
@@ -2505,8 +2505,8 @@
         <v>128</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>0x08adc0b02cc7b9ab92d629c4dda5d8ba30c376cc2a87233c62274e823f2acc3b,</v>
+        <f t="shared" si="0"/>
+        <v>0x08adc0b02cc7b9ab92d629c4dda5d8ba30c376cc2a87233c62274e823f2acc3b, // K uppercase k</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" thickBot="1">
@@ -2520,8 +2520,8 @@
         <v>129</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2704b66967d654eb68c7117614ea88aaad85d17f568b09ba61246a9b9037472a,</v>
+        <f t="shared" si="0"/>
+        <v>0x2704b66967d654eb68c7117614ea88aaad85d17f568b09ba61246a9b9037472a, // L uppercase l</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16.5" thickBot="1">
@@ -2535,8 +2535,8 @@
         <v>130</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="1"/>
-        <v>0x17454755bdb5d792b85d50f439bacea14f72154a2708c3193131397bc35b6f9f,</v>
+        <f t="shared" si="0"/>
+        <v>0x17454755bdb5d792b85d50f439bacea14f72154a2708c3193131397bc35b6f9f, // M uppercase m</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.5" thickBot="1">
@@ -2550,8 +2550,8 @@
         <v>131</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>0x279db9a32e26805bbb3311f6eaef91ee480a9979c018e813b13619d06e58f083,</v>
+        <f t="shared" si="0"/>
+        <v>0x279db9a32e26805bbb3311f6eaef91ee480a9979c018e813b13619d06e58f083, // N uppercase n</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16.5" thickBot="1">
@@ -2565,8 +2565,8 @@
         <v>132</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2eefaed7c719fc9bc9883ca01d6594e115b393888f34eeb899dc5c093c97a719,</v>
+        <f t="shared" si="0"/>
+        <v>0x2eefaed7c719fc9bc9883ca01d6594e115b393888f34eeb899dc5c093c97a719, // O uppercase o</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" thickBot="1">
@@ -2580,8 +2580,8 @@
         <v>133</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1f9b45a92bee2dd761aa1484cbc3304ebcb147549200a0666273220a4acecfa1,</v>
+        <f t="shared" si="0"/>
+        <v>0x1f9b45a92bee2dd761aa1484cbc3304ebcb147549200a0666273220a4acecfa1, // P uppercase p</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.5" thickBot="1">
@@ -2595,8 +2595,8 @@
         <v>134</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="1"/>
-        <v>0x077b1605f30c4a8537077aaae6769f06f6c422416383533dbd551d79024dd466,</v>
+        <f t="shared" si="0"/>
+        <v>0x077b1605f30c4a8537077aaae6769f06f6c422416383533dbd551d79024dd466, // Q uppercase q</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="16.5" thickBot="1">
@@ -2610,8 +2610,8 @@
         <v>135</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="1"/>
-        <v>0x21a736176abf6f07f1f42834c3871b2d669ed4fa0f698d04c7c2d9861986985c,</v>
+        <f t="shared" si="0"/>
+        <v>0x21a736176abf6f07f1f42834c3871b2d669ed4fa0f698d04c7c2d9861986985c, // R uppercase r</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="16.5" thickBot="1">
@@ -2625,8 +2625,8 @@
         <v>136</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2ba8e6d088d6e33d925299c2c302fa5d302ed02ca71937a0d74bac8c40950b62,</v>
+        <f t="shared" si="0"/>
+        <v>0x2ba8e6d088d6e33d925299c2c302fa5d302ed02ca71937a0d74bac8c40950b62, // S uppercase s</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16.5" thickBot="1">
@@ -2640,8 +2640,8 @@
         <v>137</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1e7705c06afd8c1572e5e92a642210c123c3f5985d7c72cdb1205bd074827783,</v>
+        <f t="shared" si="0"/>
+        <v>0x1e7705c06afd8c1572e5e92a642210c123c3f5985d7c72cdb1205bd074827783, // T uppercase t</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="16.5" thickBot="1">
@@ -2655,8 +2655,8 @@
         <v>138</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="1"/>
-        <v>0x12f3599cd2c7382c011484b8c3a20e2b6c37f348e8cfdeae6cdbd1885e34ad93,</v>
+        <f t="shared" si="0"/>
+        <v>0x12f3599cd2c7382c011484b8c3a20e2b6c37f348e8cfdeae6cdbd1885e34ad93, // U uppercase u</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="16.5" thickBot="1">
@@ -2670,8 +2670,8 @@
         <v>139</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>0x22ee9132c55d09fc7242206a405786885626aeda5f71380d08baae5621421b6e,</v>
+        <f t="shared" si="0"/>
+        <v>0x22ee9132c55d09fc7242206a405786885626aeda5f71380d08baae5621421b6e, // V uppercase v</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="16.5" thickBot="1">
@@ -2685,8 +2685,8 @@
         <v>140</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2961ba09ac4f854022ed58507589f4367b35871df2a2765d1bee5aded5e32b59,</v>
+        <f t="shared" si="0"/>
+        <v>0x2961ba09ac4f854022ed58507589f4367b35871df2a2765d1bee5aded5e32b59, // W uppercase w</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16.5" thickBot="1">
@@ -2700,8 +2700,8 @@
         <v>141</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1dfa6b4beb4197e649d47781456011225947205c931a1ff1a3f7560b302f542e,</v>
+        <f t="shared" si="0"/>
+        <v>0x1dfa6b4beb4197e649d47781456011225947205c931a1ff1a3f7560b302f542e, // X uppercase x</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="16.5" thickBot="1">
@@ -2715,8 +2715,8 @@
         <v>142</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2589dd87071b0706f33ccd80362dec65b042c4e347c733e73090334b9379a5e8,</v>
+        <f t="shared" si="0"/>
+        <v>0x2589dd87071b0706f33ccd80362dec65b042c4e347c733e73090334b9379a5e8, // Y uppercase y</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="16.5" thickBot="1">
@@ -2730,8 +2730,8 @@
         <v>143</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>0x1a3b00bd79bad5789ae13e4f11ca04709c685e94788f2c258e6411c8201d0186,</v>
+        <f t="shared" si="0"/>
+        <v>0x1a3b00bd79bad5789ae13e4f11ca04709c685e94788f2c258e6411c8201d0186, // Z uppercase z</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="16.5" thickBot="1">
@@ -2745,7 +2745,7 @@
         <v>144</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" ref="D60:D65" si="3">C60&amp;","&amp;" // "&amp;B60</f>
+        <f t="shared" si="0"/>
         <v>0x0d09f418d703713cdbdb76f728bb05c804c355da9ea97437de2a08fbb4614c95, // [ left square bracket</v>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
         <v>145</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0x0f01937baf69cee1bfc6d0fda869ddc154b8ab0fbf5c449fcd4f5b2f563234c5, // \ backslash</v>
       </c>
     </row>
@@ -2775,7 +2775,7 @@
         <v>146</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0x01e348e3ce89157685899df34a7b5e6ec8893e73d6b3d015fd0ab1a653b446bd, // ] right square bracket</v>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
         <v>147</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0x02fbbdfdd67fd053da748f69235e00cb779b56cec4abc46eef1aeaa5047bc6c3, // ^ caret</v>
       </c>
     </row>
@@ -2805,7 +2805,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0x06259a629d9eda880218afbdff67600e907144901aab7e6735b80bd8969cecad, // _ underscore</v>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
         <v>149</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0x15209746cea10e1113f1de0b8c66f1d573f68eaf4365dc674e5fbb58692e836f, // ` grave accent</v>
       </c>
     </row>
@@ -2835,8 +2835,8 @@
         <v>150</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="1"/>
-        <v>0x2bc4bb39989fedfe614e3ecb1459abf29c1a7c0d5f1a6198ca666a7681127a2e,</v>
+        <f t="shared" si="0"/>
+        <v>0x2bc4bb39989fedfe614e3ecb1459abf29c1a7c0d5f1a6198ca666a7681127a2e, // a lowercase a</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16.5" thickBot="1">
@@ -2850,8 +2850,8 @@
         <v>151</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D95" si="4">C67&amp;","</f>
-        <v>0x194c151fb80ae36f8738a1f1480eef6d2edd6a8d3b4ec50c7247cad56f911894,</v>
+        <f t="shared" ref="D67:D95" si="1">C67&amp;","&amp;" // "&amp;B67</f>
+        <v>0x194c151fb80ae36f8738a1f1480eef6d2edd6a8d3b4ec50c7247cad56f911894, // b lowercase b</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="16.5" thickBot="1">
@@ -2865,8 +2865,8 @@
         <v>152</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2d4829f45093c93d319654f920e83f28ea332ef2dbbda4bf4fe1a957f83cef0c,</v>
+        <f t="shared" si="1"/>
+        <v>0x2d4829f45093c93d319654f920e83f28ea332ef2dbbda4bf4fe1a957f83cef0c, // c lowercase c</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="16.5" thickBot="1">
@@ -2880,8 +2880,8 @@
         <v>153</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="4"/>
-        <v>0x14ec7c744f563a9b337121af1d454700c52b9008b4c522fe7c10bbb4229a2eaa,</v>
+        <f t="shared" si="1"/>
+        <v>0x14ec7c744f563a9b337121af1d454700c52b9008b4c522fe7c10bbb4229a2eaa, // d lowercase d</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="16.5" thickBot="1">
@@ -2895,8 +2895,8 @@
         <v>154</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2ced7a1e5259f39113165179820c949a6c1dddbd5ab404e4f876e1b94e0c686a,</v>
+        <f t="shared" si="1"/>
+        <v>0x2ced7a1e5259f39113165179820c949a6c1dddbd5ab404e4f876e1b94e0c686a, // e lowercase e</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="16.5" thickBot="1">
@@ -2910,8 +2910,8 @@
         <v>155</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="4"/>
-        <v>0x12e24f5fb500abf3c28a03ed9fb1b67f76cf8083b667cc30dbe6f5f7e72ef3f8,</v>
+        <f t="shared" si="1"/>
+        <v>0x12e24f5fb500abf3c28a03ed9fb1b67f76cf8083b667cc30dbe6f5f7e72ef3f8, // f lowercase f</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="16.5" thickBot="1">
@@ -2925,8 +2925,8 @@
         <v>156</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="4"/>
-        <v>0x26f66747c6956c29dfc148242d798aadf479493159518df4b418480f84cea098,</v>
+        <f t="shared" si="1"/>
+        <v>0x26f66747c6956c29dfc148242d798aadf479493159518df4b418480f84cea098, // g lowercase g</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="16.5" thickBot="1">
@@ -2940,8 +2940,8 @@
         <v>157</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2968e5a12a58ade28b323d4f27bc1c1ac32843c18780fcfc2206875744daf842,</v>
+        <f t="shared" si="1"/>
+        <v>0x2968e5a12a58ade28b323d4f27bc1c1ac32843c18780fcfc2206875744daf842, // h lowercase h</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="16.5" thickBot="1">
@@ -2955,8 +2955,8 @@
         <v>158</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="4"/>
-        <v>0x1331051e6aeedf737c007b0f5341ee9b1ad3db59b5e585289c99b1f3ad65fc23,</v>
+        <f t="shared" si="1"/>
+        <v>0x1331051e6aeedf737c007b0f5341ee9b1ad3db59b5e585289c99b1f3ad65fc23, // i lowercase i</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="16.5" thickBot="1">
@@ -2970,8 +2970,8 @@
         <v>159</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="4"/>
-        <v>0x08ce0afc676a95ad5bae834b7e87bae9db763dcf09d675513bfe77d3dbd597fe,</v>
+        <f t="shared" si="1"/>
+        <v>0x08ce0afc676a95ad5bae834b7e87bae9db763dcf09d675513bfe77d3dbd597fe, // j lowercase j</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="16.5" thickBot="1">
@@ -2985,8 +2985,8 @@
         <v>160</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="4"/>
-        <v>0x01d04f011534ee3bd11724f77bc6bc439785493c3ba30294ccb920185da2a9c9,</v>
+        <f t="shared" si="1"/>
+        <v>0x01d04f011534ee3bd11724f77bc6bc439785493c3ba30294ccb920185da2a9c9, // k lowercase k</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="16.5" thickBot="1">
@@ -3000,8 +3000,8 @@
         <v>161</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="4"/>
-        <v>0x058f3680b7e4899e5167e9b5bd22e94e820e0eb93decf64f8a11683c130a2284,</v>
+        <f t="shared" si="1"/>
+        <v>0x058f3680b7e4899e5167e9b5bd22e94e820e0eb93decf64f8a11683c130a2284, // l lowercase l</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="16.5" thickBot="1">
@@ -3015,8 +3015,8 @@
         <v>162</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="4"/>
-        <v>0x0fcb6a656820bac4724f84cb1dd6c77a86c0a67e66540d2d3d0c66327a81728a,</v>
+        <f t="shared" si="1"/>
+        <v>0x0fcb6a656820bac4724f84cb1dd6c77a86c0a67e66540d2d3d0c66327a81728a, // m lowercase m</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="16.5" thickBot="1">
@@ -3030,8 +3030,8 @@
         <v>163</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="4"/>
-        <v>0x02729cbddd4ec32f79556df47ee2f6ef5fb341fb98823872450fda675a06d81c,</v>
+        <f t="shared" si="1"/>
+        <v>0x02729cbddd4ec32f79556df47ee2f6ef5fb341fb98823872450fda675a06d81c, // n lowercase n</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="16.5" thickBot="1">
@@ -3045,8 +3045,8 @@
         <v>164</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="4"/>
-        <v>0x0c961db6c8d4454cef7c0f1ba8d07169eb512a9806066132325e701ff8f6fe22,</v>
+        <f t="shared" si="1"/>
+        <v>0x0c961db6c8d4454cef7c0f1ba8d07169eb512a9806066132325e701ff8f6fe22, // o lowercase o</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="16.5" thickBot="1">
@@ -3060,8 +3060,8 @@
         <v>165</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="4"/>
-        <v>0x201a8ea4e78ecc2e6f5c55b1a3e9e430db82c8fc6cbf46af4674d3c956437ef8,</v>
+        <f t="shared" si="1"/>
+        <v>0x201a8ea4e78ecc2e6f5c55b1a3e9e430db82c8fc6cbf46af4674d3c956437ef8, // p lowercase p</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="16.5" thickBot="1">
@@ -3075,8 +3075,8 @@
         <v>166</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2cd078c0879ecda31e2267bd9ae5ff086c10ae1cc1a75120a5519685f4dfaddf,</v>
+        <f t="shared" si="1"/>
+        <v>0x2cd078c0879ecda31e2267bd9ae5ff086c10ae1cc1a75120a5519685f4dfaddf, // q lowercase q</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="16.5" thickBot="1">
@@ -3090,8 +3090,8 @@
         <v>167</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="4"/>
-        <v>0x072e3e9c8cc55501d578de583573bf146f8bc54938c7a811ea053001a2210523,</v>
+        <f t="shared" si="1"/>
+        <v>0x072e3e9c8cc55501d578de583573bf146f8bc54938c7a811ea053001a2210523, // r lowercase r</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="16.5" thickBot="1">
@@ -3105,8 +3105,8 @@
         <v>168</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2ac4e33de9876873c93bc790c1b3ed01800ea98459dc786d921df830755eee1e,</v>
+        <f t="shared" si="1"/>
+        <v>0x2ac4e33de9876873c93bc790c1b3ed01800ea98459dc786d921df830755eee1e, // s lowercase s</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="16.5" thickBot="1">
@@ -3120,8 +3120,8 @@
         <v>169</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="4"/>
-        <v>0x1be43ae9ae5f0b01a507385db6f27e33e1cf5134ec652254362a5d34e56c09a5,</v>
+        <f t="shared" si="1"/>
+        <v>0x1be43ae9ae5f0b01a507385db6f27e33e1cf5134ec652254362a5d34e56c09a5, // t lowercase t</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="16.5" thickBot="1">
@@ -3135,8 +3135,8 @@
         <v>170</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2610f7adaf1126426670b6849d593889024ce9749f7edf747b8c44af0022a545,</v>
+        <f t="shared" si="1"/>
+        <v>0x2610f7adaf1126426670b6849d593889024ce9749f7edf747b8c44af0022a545, // u lowercase u</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="16.5" thickBot="1">
@@ -3150,8 +3150,8 @@
         <v>171</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="4"/>
-        <v>0x063841d8f34cac19fd660c9e470744b301c3dd193dec844672a67cd6a861bb94,</v>
+        <f t="shared" si="1"/>
+        <v>0x063841d8f34cac19fd660c9e470744b301c3dd193dec844672a67cd6a861bb94, // v lowercase v</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="16.5" thickBot="1">
@@ -3165,8 +3165,8 @@
         <v>172</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="4"/>
-        <v>0x27b92c81069a4b05563667e882ad508c99b5c6e1ae1701afe207df4ef65f5fb9,</v>
+        <f t="shared" si="1"/>
+        <v>0x27b92c81069a4b05563667e882ad508c99b5c6e1ae1701afe207df4ef65f5fb9, // w lowercase w</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="16.5" thickBot="1">
@@ -3180,8 +3180,8 @@
         <v>173</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2ae5fa247a03778d66f20d927c12f565ec886a809aacfc5ebc75ac7e7c899380,</v>
+        <f t="shared" si="1"/>
+        <v>0x2ae5fa247a03778d66f20d927c12f565ec886a809aacfc5ebc75ac7e7c899380, // x lowercase x</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="16.5" thickBot="1">
@@ -3195,8 +3195,8 @@
         <v>174</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="4"/>
-        <v>0x29bb1950faffed939e244e9eb11f20cfeeef657f2a62aaebccccb9369edb53b7,</v>
+        <f t="shared" si="1"/>
+        <v>0x29bb1950faffed939e244e9eb11f20cfeeef657f2a62aaebccccb9369edb53b7, // y lowercase y</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="16.5" thickBot="1">
@@ -3210,8 +3210,8 @@
         <v>175</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="4"/>
-        <v>0x2a902a1f449d7349ee0ea36e260d19a1a63fbe9ae3e5d7524540189de9eaf9cd,</v>
+        <f t="shared" si="1"/>
+        <v>0x2a902a1f449d7349ee0ea36e260d19a1a63fbe9ae3e5d7524540189de9eaf9cd, // z lowercase z</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="16.5" thickBot="1">
@@ -3225,7 +3225,7 @@
         <v>176</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" ref="D92:D95" si="5">C92&amp;","&amp;" // "&amp;B92</f>
+        <f t="shared" si="1"/>
         <v>0x11fef81a0260cd6e7df99bc73b229ef3721b00d13896312a7d9fe3eebc7a96a5, // { left curly brace</v>
       </c>
     </row>
@@ -3240,7 +3240,7 @@
         <v>177</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0x09bfbd4baddb71f67d791a652163f5692659e4f588f12f48030799b9b5090b57, // | vertical bar</v>
       </c>
     </row>
@@ -3255,7 +3255,7 @@
         <v>178</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0x23caca35a8635bda4f9c5d595650cde82a667ac26832dfeb86154a45041dc6ce, // } right curly brace</v>
       </c>
     </row>
@@ -3270,7 +3270,7 @@
         <v>179</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0x2c4c41588a752611fcdafa8762309149af9cb49fd71a7eec360f5332a7c0df2f, // ~ tilde</v>
       </c>
     </row>

</xml_diff>